<commit_message>
update utils create excel file and add telegram bot
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -16,19 +16,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Quantity</t>
+    <t>Название</t>
+  </si>
+  <si>
+    <t>Цена</t>
+  </si>
+  <si>
+    <t>Количесво</t>
+  </si>
+  <si>
+    <t>Цена за эти товары</t>
   </si>
   <si>
     <t>candle</t>
-  </si>
-  <si>
-    <t>sylvia-breitenberg</t>
   </si>
 </sst>
 </file>
@@ -337,6 +337,12 @@
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="true" max="1" min="1" width="8"/>
+    <col customWidth="true" max="2" min="2" width="14"/>
+    <col customWidth="true" max="3" min="3" width="20"/>
+    <col customWidth="true" max="4" min="4" width="15"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -348,27 +354,22 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>500</v>
       </c>
       <c r="C2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>615</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>3000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add send product excel file and add method sedn document bot service
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -366,10 +366,10 @@
         <v>500</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>3000</v>
+        <v>6000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add send order for cannel telegram
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Название</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>Цена за эти товары</t>
+  </si>
+  <si>
+    <t>Цена за все экраны</t>
   </si>
   <si>
     <t>candle</t>
@@ -338,10 +341,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="8"/>
-    <col customWidth="true" max="2" min="2" width="14"/>
-    <col customWidth="true" max="3" min="3" width="20"/>
-    <col customWidth="true" max="4" min="4" width="15"/>
+    <col customWidth="true" max="1" min="1" width="16"/>
+    <col customWidth="true" max="2" min="2" width="22"/>
+    <col customWidth="true" max="3" min="3" width="28"/>
+    <col customWidth="true" max="4" min="4" width="23"/>
+    <col customWidth="true" max="5" min="5" width="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -357,19 +361,27 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>500</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>6000</v>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="E3">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor bot,add botkit and add bot to app folder
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Название</t>
   </si>
@@ -28,10 +28,13 @@
     <t>Цена за эти товары</t>
   </si>
   <si>
-    <t>Цена за все экраны</t>
+    <t>Цена за все товары</t>
   </si>
   <si>
     <t>candle</t>
+  </si>
+  <si>
+    <t>sylvia-breitenberg</t>
   </si>
 </sst>
 </file>
@@ -341,9 +344,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="16"/>
+    <col customWidth="true" max="1" min="1" width="28"/>
     <col customWidth="true" max="2" min="2" width="22"/>
-    <col customWidth="true" max="3" min="3" width="28"/>
+    <col customWidth="true" max="3" min="3" width="40"/>
     <col customWidth="true" max="4" min="4" width="23"/>
     <col customWidth="true" max="5" min="5" width="10"/>
   </cols>
@@ -373,15 +376,29 @@
         <v>500</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>1000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="3">
-      <c r="E3">
-        <v>1000</v>
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>615</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>3075</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="E4">
+        <v>4575</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor bot functions(need more refactor)
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Название</t>
   </si>
@@ -31,10 +31,7 @@
     <t>Цена за все товары</t>
   </si>
   <si>
-    <t>candle</t>
-  </si>
-  <si>
-    <t>sylvia-breitenberg</t>
+    <t>tre-wunsch</t>
   </si>
 </sst>
 </file>
@@ -344,10 +341,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="28"/>
-    <col customWidth="true" max="2" min="2" width="22"/>
-    <col customWidth="true" max="3" min="3" width="40"/>
-    <col customWidth="true" max="4" min="4" width="23"/>
+    <col customWidth="true" max="1" min="1" width="20"/>
+    <col customWidth="true" max="2" min="2" width="23"/>
+    <col customWidth="true" max="3" min="3" width="32"/>
+    <col customWidth="true" max="4" min="4" width="24"/>
     <col customWidth="true" max="5" min="5" width="10"/>
   </cols>
   <sheetData>
@@ -373,32 +370,18 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>500</v>
+        <v>1791</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>1500</v>
+        <v>21492</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>615</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>3075</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="E4">
-        <v>4575</v>
+      <c r="E3">
+        <v>21492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add delete category resolver
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Название</t>
   </si>
@@ -31,7 +31,22 @@
     <t>Цена за все товары</t>
   </si>
   <si>
-    <t>tre-wunsch</t>
+    <t>jon-wyman</t>
+  </si>
+  <si>
+    <t>ciara-gislason</t>
+  </si>
+  <si>
+    <t>candle</t>
+  </si>
+  <si>
+    <t>white-candle</t>
+  </si>
+  <si>
+    <t>mariam-king</t>
+  </si>
+  <si>
+    <t>johnny-cummings</t>
   </si>
 </sst>
 </file>
@@ -341,10 +356,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="20"/>
+    <col customWidth="true" max="1" min="1" width="25"/>
     <col customWidth="true" max="2" min="2" width="23"/>
-    <col customWidth="true" max="3" min="3" width="32"/>
-    <col customWidth="true" max="4" min="4" width="24"/>
+    <col customWidth="true" max="3" min="3" width="37"/>
+    <col customWidth="true" max="4" min="4" width="23"/>
     <col customWidth="true" max="5" min="5" width="10"/>
   </cols>
   <sheetData>
@@ -370,18 +385,88 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1791</v>
+        <v>2116</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>21492</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="3">
-      <c r="E3">
-        <v>21492</v>
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>1738</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1738</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>500</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>1000</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>2309</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>1473</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="E8">
+        <v>9136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add delete candle by id
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Название</t>
   </si>
@@ -31,22 +31,10 @@
     <t>Цена за все товары</t>
   </si>
   <si>
-    <t>jon-wyman</t>
+    <t>esther-okuneva</t>
   </si>
   <si>
     <t>ciara-gislason</t>
-  </si>
-  <si>
-    <t>candle</t>
-  </si>
-  <si>
-    <t>white-candle</t>
-  </si>
-  <si>
-    <t>mariam-king</t>
-  </si>
-  <si>
-    <t>johnny-cummings</t>
   </si>
 </sst>
 </file>
@@ -356,9 +344,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="25"/>
+    <col customWidth="true" max="1" min="1" width="24"/>
     <col customWidth="true" max="2" min="2" width="23"/>
-    <col customWidth="true" max="3" min="3" width="37"/>
+    <col customWidth="true" max="3" min="3" width="36"/>
     <col customWidth="true" max="4" min="4" width="23"/>
     <col customWidth="true" max="5" min="5" width="10"/>
   </cols>
@@ -385,13 +373,13 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>2116</v>
+        <v>1562</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>2116</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="3">
@@ -409,64 +397,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>500</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>1000</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>2309</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>2309</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>1473</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1473</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="E8">
-        <v>9136</v>
+      <c r="E4">
+        <v>3300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>